<commit_message>
Objectif 2 : prépa pour calcul de taux par_p_par_c
</commit_message>
<xml_diff>
--- a/Légende - Plan de plaque MTECC.xlsx
+++ b/Légende - Plan de plaque MTECC.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adele\Bureau\INEM\Code-MTECC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MTECC data Splicing mut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CD9330-35E3-4BAA-9BCD-120D485A241F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{54FDE8CD-E475-4B72-9A64-0957BC835E0C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Px</t>
   </si>
@@ -59,9 +58,6 @@
     <t>CODE</t>
   </si>
   <si>
-    <t>WT</t>
-  </si>
-  <si>
     <t>Wild Type</t>
   </si>
   <si>
@@ -74,9 +70,6 @@
     <t>PredictCDdec162k</t>
   </si>
   <si>
-    <t>Exemple description si patient est un mutant : "M1_P1_T2"</t>
-  </si>
-  <si>
     <t>Patient</t>
   </si>
   <si>
@@ -89,29 +82,6 @@
     <t>F508del/F508del</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Plaque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t>Ax</t>
   </si>
   <si>
@@ -136,23 +106,45 @@
     <t>Api</t>
   </si>
   <si>
-    <t>Exemple description si patient est un WT : "WT_P1_C1_A1"</t>
+    <t>WTx</t>
+  </si>
+  <si>
+    <t>Exemple description si patient est un WT : "WT1_NomPrénom_ctrl"</t>
+  </si>
+  <si>
+    <t>Exemple description si patient est un WT : "WT1_NomPrénom_vx661-vx445_vx770-Api"</t>
+  </si>
+  <si>
+    <t>Exemple description si patient est un mutant : "M1_Nomprénom_ctrl_vx770-Api"</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>NomPrénom</t>
+  </si>
+  <si>
+    <t>vx661-vx445</t>
+  </si>
+  <si>
+    <t>Codage de la colonne "Description " pour MTECC</t>
+  </si>
+  <si>
+    <t>Plaque MTECC</t>
+  </si>
+  <si>
+    <t>vx770-Api</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -165,8 +157,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +194,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -188,16 +215,257 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -273,53 +541,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCF72864-CF5F-42BA-B7B6-FF22E6795134}" name="Tableau1" displayName="Tableau1" ref="A4:B6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A4:B6" xr:uid="{FCF72864-CF5F-42BA-B7B6-FF22E6795134}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A4:B6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A4:B6"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FC6AE61C-451D-4E30-959F-E4F19A5C8CED}" name="Px" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{7B1E72E5-AEC3-4C5B-8AD2-DAC766F0EF35}" name="Patients" dataDxfId="14"/>
+    <tableColumn id="1" name="Px" dataDxfId="15"/>
+    <tableColumn id="2" name="Patients" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{920AD4C1-5535-478F-ABCE-105913E2438D}" name="Tableau13" displayName="Tableau13" ref="D4:E7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="D4:E7" xr:uid="{920AD4C1-5535-478F-ABCE-105913E2438D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="D4:E7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="D4:E7"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FF68403F-A5F2-4CF4-B626-BA6472391F53}" name="Mx" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C7261F6A-7C13-439A-A16C-A0891FB7DA5A}" name="Mutations" dataDxfId="10"/>
+    <tableColumn id="1" name="Mx" dataDxfId="11"/>
+    <tableColumn id="2" name="Mutations" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3DF5C5E-0F60-4DD2-A9E4-F1A2F50B5B98}" name="Tableau14" displayName="Tableau14" ref="G4:G8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="G4:G8" xr:uid="{D3DF5C5E-0F60-4DD2-A9E4-F1A2F50B5B98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau14" displayName="Tableau14" ref="G4:G8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="G4:G8"/>
   <tableColumns count="1">
-    <tableColumn id="2" xr3:uid="{A8199F50-F3BB-43BB-A327-65AA340FE4F9}" name="Chronique" dataDxfId="7"/>
+    <tableColumn id="2" name="Chronique" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CBC7F263-D96D-47C6-8EEE-DD66D3E05B83}" name="Tableau145" displayName="Tableau145" ref="A11:B18" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A11:B18" xr:uid="{CBC7F263-D96D-47C6-8EEE-DD66D3E05B83}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau145" displayName="Tableau145" ref="A11:B18" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A11:B18"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6EDFDF9B-A88C-42D8-B6D9-E6EE302B21C8}" name="CODE" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4D433FA1-D765-4928-B0CF-FE662887FF39}" name="Correspond à…" dataDxfId="3"/>
+    <tableColumn id="1" name="CODE" dataDxfId="4"/>
+    <tableColumn id="2" name="Correspond à…" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E8EAD240-A367-4FAD-98C4-A55CE542C264}" name="Tableau147" displayName="Tableau147" ref="G10:G13" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="G10:G13" xr:uid="{E8EAD240-A367-4FAD-98C4-A55CE542C264}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau147" displayName="Tableau147" ref="I4:I7" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="I4:I7"/>
   <tableColumns count="1">
-    <tableColumn id="2" xr3:uid="{2FCAA9A0-3890-4E87-961B-E993EAA2A449}" name="Accute" dataDxfId="0"/>
+    <tableColumn id="2" name="Accute" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -641,66 +909,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7373A70B-B4D9-4AD4-A0DC-E9278A0F0842}">
-  <dimension ref="A1:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="1"/>
-    <col min="2" max="2" width="23.26953125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.90625" style="1"/>
-    <col min="5" max="5" width="15.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" style="1"/>
-    <col min="7" max="7" width="13.36328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.90625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="23.25" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.875" style="1"/>
+    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
+      <c r="A1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="22"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="25"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickBot="1">
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="28"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,11 +986,14 @@
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -729,118 +1004,200 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H6"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="G7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="H8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="15" thickBot="1"/>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1">
+      <c r="E10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" thickBot="1">
       <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15" thickBot="1">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="D18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="F19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K3"/>
+  <mergeCells count="2">
+    <mergeCell ref="E10:K10"/>
+    <mergeCell ref="A1:L3"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="5">
     <tablePart r:id="rId1"/>

</xml_diff>